<commit_message>
feat(ocr, ein/ausgang): OCR-gestützte Erfassung, DB-Abgleich und Druck-Workflow
OCR robuster: 0/90/180/270° (PSM 6) + Feinsweeps ±4/8/12° (PSM 11 + Otsu), Bounding-Boxes im Stream
Webcam: DirectShow (CAP_DSHOW) + MJPG, max. 720p @ 30 FPS, OCR auf 960px Breite skaliert
Wareneingang/-ausgang: OCR-Treffer gegen Excel (Status "0") matchen und in Treeviews einfügen
Warenausgang unterstützt zusätzlich Spalte Empfänger aus Excel
Access-DB (Artikeldatenbank): Karton/Beutel per pyodbc nachladen (Treiber-Check), Cache + asynchrones Update in Tabelle
Drucken (beide Seiten): Artikelnummer/Menge in Konsole, Excel-Status 0→1, UI-Status auf ✅; bereits ✅ → Zeile entfernen
Navigation/Binds: OCR nur auf Eingangs-/Ausgangsseiten aktiv; Enter löst Drucken aus
Sonstiges: Tesseract-Pfad gesetzt; Debug-Ausgaben (Interpreter/ODBC/DB-Pfad, F9 zeigt Datenvorschau)
</commit_message>
<xml_diff>
--- a/ausgang/test_02_Ausgang.xlsx
+++ b/ausgang/test_02_Ausgang.xlsx
@@ -1,76 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="122211" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>Artikelnummer</t>
-  </si>
-  <si>
-    <t>Menge</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>KL5011</t>
-  </si>
-  <si>
-    <t>KL5012</t>
-  </si>
-  <si>
-    <t>KL5013</t>
-  </si>
-  <si>
-    <t>KL5014</t>
-  </si>
-  <si>
-    <t>KL5015</t>
-  </si>
-  <si>
-    <t>KL5016</t>
-  </si>
-  <si>
-    <t>Empfänger</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>HUN</t>
-  </si>
-  <si>
-    <t>3 HUN; 3 PL</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -393,113 +409,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col width="15.77734375" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Artikelnummer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Menge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Empfänger</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AS5011</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>KL5012</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HUN</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>KL5013</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HUN</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KL5014</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HUN</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>KL5015</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3 HUN; 3 PL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KL5016</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>